<commit_message>
Strong scaling avec plus gros domaine
</commit_message>
<xml_diff>
--- a/Analyse .out/ScalabilityShallow.xlsx
+++ b/Analyse .out/ScalabilityShallow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9be20e56d8dc8fd/Documents/GitHub/Projet-HPC/Analyse .out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{07A788C6-E1AB-4A6F-A8A8-DB69971995BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A430AE3-7B8A-4297-B9F4-373EFADAFE21}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{07A788C6-E1AB-4A6F-A8A8-DB69971995BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D03B1CDE-7AA6-4BD1-950C-8918676FF935}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="3" xr2:uid="{F37CA3FF-E8FD-40D0-995D-F29E9880726D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="2" xr2:uid="{F37CA3FF-E8FD-40D0-995D-F29E9880726D}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong OpenMP" sheetId="4" r:id="rId1"/>
@@ -655,22 +655,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6428170918693974</c:v>
+                  <c:v>1.592547270549898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.407159784987114</c:v>
+                  <c:v>1.9449801511644749</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4756499951189355</c:v>
+                  <c:v>1.9057781536554423</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.650454915259941</c:v>
+                  <c:v>2.1182170417861514</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.001944000668221</c:v>
+                  <c:v>9.0035264246498343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.063378915930123</c:v>
+                  <c:v>48.163310120291086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,22 +872,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8214085459346987</c:v>
+                  <c:v>0.79627363527494899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60178994624677851</c:v>
+                  <c:v>0.48624503779111872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0594562493898669</c:v>
+                  <c:v>0.23822226920693029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97815343220374629</c:v>
+                  <c:v>0.13238856511163447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81256075002088191</c:v>
+                  <c:v>0.28136020077030732</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43849029556140817</c:v>
+                  <c:v>0.75255172062954823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,22 +1480,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>13.3470333333333</c:v>
+                  <c:v>83.885300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.94969666666666</c:v>
+                  <c:v>52.741325000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6680979999999901</c:v>
+                  <c:v>10.39695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92075016666666598</c:v>
+                  <c:v>5.0351224999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.6880666666666</c:v>
+                  <c:v>49.744900000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75.660216666666599</c:v>
+                  <c:v>94.252200000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,22 +1571,22 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.5116300000000003</c:v>
+                  <c:v>41.3832375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.69161875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.345809375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1729046875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.58645234375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.293226171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2070,19 +2070,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.96110964878833816</c:v>
+                  <c:v>0.97784167434606939</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6218441680010884</c:v>
+                  <c:v>1.5692907790996906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.399876161104826</c:v>
+                  <c:v>12.844617275558804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.935300785133126</c:v>
+                  <c:v>31.461649136544885</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34371927997135543</c:v>
+                  <c:v>1.7526321306282173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2271,19 +2271,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.24027741219708454</c:v>
+                  <c:v>0.24446041858651735</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20273052100013605</c:v>
+                  <c:v>0.19616134738746133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89999226006905164</c:v>
+                  <c:v>0.80278857972242523</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8104781495354102</c:v>
+                  <c:v>0.98317653551702766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3706137495524286E-3</c:v>
+                  <c:v>2.7384877041065896E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2888,22 +2888,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.97574192517188829</c:v>
+                  <c:v>0.98666244264489722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6382084180151122</c:v>
+                  <c:v>1.5692907790996906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8072511327272602</c:v>
+                  <c:v>7.960649517406547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.144184243970644</c:v>
+                  <c:v>16.437827480860694</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31239779249377569</c:v>
+                  <c:v>1.6638183009715568</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17212824088749432</c:v>
+                  <c:v>0.8781383882816528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3095,22 +3095,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.48787096258594415</c:v>
+                  <c:v>0.49333122132244861</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40955210450377805</c:v>
+                  <c:v>0.39232269477492265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97590639159090753</c:v>
+                  <c:v>0.99508118967581838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88401151524816524</c:v>
+                  <c:v>1.0273642175537934</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7624310154304905E-3</c:v>
+                  <c:v>5.199432190536115E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6895037638670987E-3</c:v>
+                  <c:v>1.3720912316900825E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3700,22 +3700,22 @@
             <c:numRef>
               <c:f>'Strong Hybrid'!$H$4:$H$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>13.550233333333299</c:v>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>84.641999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0299083333333297</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.90440083333333299</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.50214416666666595</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>37.889233333333301</c:v>
+                  <c:v>52.741325000000003</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>6.44367</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>2.6307100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000">
+                  <c:v>47.2241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3791,19 +3791,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.69161875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.345809375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1729046875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.58645234375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.293226171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4271,16 +4271,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.9047666666666</c:v>
+                  <c:v>84.36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3170016666666609</c:v>
+                  <c:v>52.997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53570533333333303</c:v>
+                  <c:v>6.4591700000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.302153</c:v>
+                  <c:v>1.51515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4356,16 +4356,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.345809375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1729046875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.58645234375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.293226171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8614,25 +8614,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.250050000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9273949999999997</c:v>
+                  <c:v>51.646850000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4102183333333302</c:v>
+                  <c:v>42.288375000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5365500000000001</c:v>
+                  <c:v>43.158250000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.83213300000000001</c:v>
+                  <c:v>38.82985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.50085716666666602</c:v>
+                  <c:v>9.1353150000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46406599999999898</c:v>
+                  <c:v>1.7077325000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8711,25 +8711,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.250050000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5116300000000003</c:v>
+                  <c:v>41.125025000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.5625125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.28125625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1406281250000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.5703140625000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.28515703125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9955,22 +9955,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1287390378448574</c:v>
+                  <c:v>1.5331343211248074</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.225045784203517</c:v>
+                  <c:v>1.9238427712675135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.663761600160063</c:v>
+                  <c:v>5.2690209940730757</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0284859927115626</c:v>
+                  <c:v>14.554645804725435</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.608042961310264</c:v>
+                  <c:v>30.58227500754796</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.345293846329383</c:v>
+                  <c:v>47.380698641658121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10172,22 +10172,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0643695189224287</c:v>
+                  <c:v>0.7665671605624037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0562614460508792</c:v>
+                  <c:v>0.48096069281687837</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95797020002000788</c:v>
+                  <c:v>0.65862762425913446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56428037454447266</c:v>
+                  <c:v>0.90966536279533972</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48775134254094576</c:v>
+                  <c:v>0.95569609398587374</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42727021634889661</c:v>
+                  <c:v>0.74032341627590814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10447,7 +10447,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1000000000000001"/>
-          <c:min val="-"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -10787,25 +10787,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.250050000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1178283333333301</c:v>
+                  <c:v>53.648299999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.082395</c:v>
+                  <c:v>42.753</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.69933</c:v>
+                  <c:v>15.61012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4424633333333301</c:v>
+                  <c:v>5.6511199999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83439416666666599</c:v>
+                  <c:v>2.6894680000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.476252333333333</c:v>
+                  <c:v>1.73594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10884,25 +10884,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.250050000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5116300000000003</c:v>
+                  <c:v>41.125025000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.5625125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.28125625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1406281250000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.5703140625000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.28515703125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11367,25 +11367,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.766475</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8162839999999996</c:v>
+                  <c:v>52.150500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9726299999999899</c:v>
+                  <c:v>21.254525000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5325120000000001</c:v>
+                  <c:v>9.6265000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80468039999999996</c:v>
+                  <c:v>4.7676224999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41275420000000002</c:v>
+                  <c:v>2.4055300000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2284128</c:v>
+                  <c:v>1.3127530000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11464,25 +11464,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.766475</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5116300000000003</c:v>
+                  <c:v>41.3832375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.69161875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.345809375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1729046875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.58645234375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.293226171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11967,22 +11967,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6661702670987903</c:v>
+                  <c:v>1.5870696349987057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3810565055186972</c:v>
+                  <c:v>3.8940637346635598</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4979823975277196</c:v>
+                  <c:v>8.5977743728250147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.184388236621647</c:v>
+                  <c:v>17.360115025885545</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.552095654023631</c:v>
+                  <c:v>34.406752358108193</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.016331834292998</c:v>
+                  <c:v>63.048018172497031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12186,22 +12186,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83308513354939517</c:v>
+                  <c:v>0.79353481749935284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0952641263796743</c:v>
+                  <c:v>0.97351593366588995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0622477996909649</c:v>
+                  <c:v>1.0747217966031268</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0115242647888529</c:v>
+                  <c:v>1.0850071891178465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98600298918823848</c:v>
+                  <c:v>1.075211011190881</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8908801849108281</c:v>
+                  <c:v>0.98512528394526611</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12815,25 +12815,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.67863890533738</c:v>
+                  <c:v>1.5937305004968763</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3566835939329467</c:v>
+                  <c:v>3.8913011584536652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4651164604650617</c:v>
+                  <c:v>8.609546777252616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.123291755062585</c:v>
+                  <c:v>17.441213477746796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.655031938786426</c:v>
+                  <c:v>34.411186094061023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.703480128741624</c:v>
+                  <c:v>63.32723683002235</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.939889336710877</c:v>
+                  <c:v>118.2470315356139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13046,25 +13046,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83931945266869001</c:v>
+                  <c:v>0.79686525024843813</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0891708984832367</c:v>
+                  <c:v>0.9728252896134163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0581395575581327</c:v>
+                  <c:v>1.076193347156577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0077057346914116</c:v>
+                  <c:v>1.0900758423591748</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9892197480870758</c:v>
+                  <c:v>1.075349565439407</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90161687701158788</c:v>
+                  <c:v>0.98948807546909923</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70265538544305373</c:v>
+                  <c:v>0.92380493387198359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13658,28 +13658,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.753500000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7582259999999996</c:v>
+                  <c:v>51.924399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9892599999999998</c:v>
+                  <c:v>21.266279999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.538462</c:v>
+                  <c:v>9.6118299999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80772960000000005</c:v>
+                  <c:v>4.7447100000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.411412</c:v>
+                  <c:v>2.4048430000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.225692799999999</c:v>
+                  <c:v>1.3067599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1447996</c:v>
+                  <c:v>0.69983574999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13761,28 +13761,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13.023260000000001</c:v>
+                  <c:v>82.753500000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5116300000000003</c:v>
+                  <c:v>41.376750000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2558150000000001</c:v>
+                  <c:v>20.688375000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6279075000000001</c:v>
+                  <c:v>10.3441875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81395375000000003</c:v>
+                  <c:v>5.1720937500000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40697687500000002</c:v>
+                  <c:v>2.5860468750000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20348843750000001</c:v>
+                  <c:v>1.2930234375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10174421875</c:v>
+                  <c:v>0.64651171875000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14265,16 +14265,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.93660399431370511</c:v>
+                  <c:v>0.98111041963015644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5658599723738595</c:v>
+                  <c:v>1.5617200030190388</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.310491588659453</c:v>
+                  <c:v>12.813794187178848</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.101541272136963</c:v>
+                  <c:v>54.625928125928127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14460,16 +14460,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.11707549928921314</c:v>
+                  <c:v>0.12263880245376955</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7866248273366221E-2</c:v>
+                  <c:v>9.7607500188689925E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75970286214560789</c:v>
+                  <c:v>0.400431068349339</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67346158237714004</c:v>
+                  <c:v>0.85353012696762698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26829,6 +26829,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -27152,7 +27156,7 @@
   <dimension ref="B2:N11"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27235,11 +27239,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>13.023260000000001</v>
+        <v>82.250050000000002</v>
       </c>
       <c r="D5" s="5">
         <f>C5</f>
-        <v>13.023260000000001</v>
+        <v>82.250050000000002</v>
       </c>
       <c r="E5" s="6">
         <f>C5/C5</f>
@@ -27257,11 +27261,11 @@
         <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>13.023260000000001</v>
+        <v>82.250050000000002</v>
       </c>
       <c r="K5" s="5">
         <f>J5</f>
-        <v>13.023260000000001</v>
+        <v>82.250050000000002</v>
       </c>
       <c r="L5" s="6">
         <f>J5/J5</f>
@@ -27281,15 +27285,15 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>7.9273949999999997</v>
+        <v>51.646850000000001</v>
       </c>
       <c r="D6" s="5">
         <f>D5/2</f>
-        <v>6.5116300000000003</v>
+        <v>41.125025000000001</v>
       </c>
       <c r="E6" s="6">
         <f>C5/C6</f>
-        <v>1.6428170918693974</v>
+        <v>1.592547270549898</v>
       </c>
       <c r="F6" s="6">
         <f>B6/B5</f>
@@ -27297,21 +27301,21 @@
       </c>
       <c r="G6" s="7">
         <f t="shared" ref="G6:G11" si="0">E6/F6</f>
-        <v>0.8214085459346987</v>
+        <v>0.79627363527494899</v>
       </c>
       <c r="I6" s="4">
         <v>2</v>
       </c>
       <c r="J6" s="5">
-        <v>6.1178283333333301</v>
+        <v>53.648299999999999</v>
       </c>
       <c r="K6" s="5">
         <f>K5/2</f>
-        <v>6.5116300000000003</v>
+        <v>41.125025000000001</v>
       </c>
       <c r="L6" s="6">
         <f>J5/J6</f>
-        <v>2.1287390378448574</v>
+        <v>1.5331343211248074</v>
       </c>
       <c r="M6" s="6">
         <f>I6/I5</f>
@@ -27319,7 +27323,7 @@
       </c>
       <c r="N6" s="7">
         <f t="shared" ref="N6:N11" si="1">L6/M6</f>
-        <v>1.0643695189224287</v>
+        <v>0.7665671605624037</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="16" x14ac:dyDescent="0.4">
@@ -27327,15 +27331,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="5">
-        <v>5.4102183333333302</v>
+        <v>42.288375000000002</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" ref="D7:D11" si="2">D6/2</f>
-        <v>3.2558150000000001</v>
+        <v>20.5625125</v>
       </c>
       <c r="E7" s="6">
         <f>C5/C7</f>
-        <v>2.407159784987114</v>
+        <v>1.9449801511644749</v>
       </c>
       <c r="F7" s="6">
         <f>B7/B5</f>
@@ -27343,21 +27347,21 @@
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>0.60178994624677851</v>
+        <v>0.48624503779111872</v>
       </c>
       <c r="I7" s="4">
         <v>4</v>
       </c>
       <c r="J7" s="5">
-        <v>3.082395</v>
+        <v>42.753</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ref="K7:K11" si="3">K6/2</f>
-        <v>3.2558150000000001</v>
+        <v>20.5625125</v>
       </c>
       <c r="L7" s="6">
         <f>J5/J7</f>
-        <v>4.225045784203517</v>
+        <v>1.9238427712675135</v>
       </c>
       <c r="M7" s="6">
         <f>I7/I5</f>
@@ -27365,7 +27369,7 @@
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>1.0562614460508792</v>
+        <v>0.48096069281687837</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="16" x14ac:dyDescent="0.4">
@@ -27373,15 +27377,15 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>1.5365500000000001</v>
+        <v>43.158250000000002</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="2"/>
-        <v>1.6279075000000001</v>
+        <v>10.28125625</v>
       </c>
       <c r="E8" s="6">
         <f>C5/C8</f>
-        <v>8.4756499951189355</v>
+        <v>1.9057781536554423</v>
       </c>
       <c r="F8" s="6">
         <f>B8/B5</f>
@@ -27389,21 +27393,21 @@
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>1.0594562493898669</v>
+        <v>0.23822226920693029</v>
       </c>
       <c r="I8" s="4">
         <v>8</v>
       </c>
       <c r="J8" s="5">
-        <v>1.69933</v>
+        <v>15.61012</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="3"/>
-        <v>1.6279075000000001</v>
+        <v>10.28125625</v>
       </c>
       <c r="L8" s="6">
         <f>J5/J8</f>
-        <v>7.663761600160063</v>
+        <v>5.2690209940730757</v>
       </c>
       <c r="M8" s="6">
         <f>I8/I5</f>
@@ -27411,7 +27415,7 @@
       </c>
       <c r="N8" s="7">
         <f t="shared" si="1"/>
-        <v>0.95797020002000788</v>
+        <v>0.65862762425913446</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.4">
@@ -27419,15 +27423,15 @@
         <v>16</v>
       </c>
       <c r="C9" s="5">
-        <v>0.83213300000000001</v>
+        <v>38.82985</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="2"/>
-        <v>0.81395375000000003</v>
+        <v>5.1406281250000001</v>
       </c>
       <c r="E9" s="6">
         <f>C5/C9</f>
-        <v>15.650454915259941</v>
+        <v>2.1182170417861514</v>
       </c>
       <c r="F9" s="6">
         <f>B9/B5</f>
@@ -27435,21 +27439,21 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>0.97815343220374629</v>
+        <v>0.13238856511163447</v>
       </c>
       <c r="I9" s="4">
         <v>16</v>
       </c>
       <c r="J9" s="5">
-        <v>1.4424633333333301</v>
+        <v>5.6511199999999997</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="3"/>
-        <v>0.81395375000000003</v>
+        <v>5.1406281250000001</v>
       </c>
       <c r="L9" s="6">
         <f>J5/J9</f>
-        <v>9.0284859927115626</v>
+        <v>14.554645804725435</v>
       </c>
       <c r="M9" s="6">
         <f>I9/I5</f>
@@ -27457,7 +27461,7 @@
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>0.56428037454447266</v>
+        <v>0.90966536279533972</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="16" x14ac:dyDescent="0.4">
@@ -27465,15 +27469,15 @@
         <v>32</v>
       </c>
       <c r="C10" s="5">
-        <v>0.50085716666666602</v>
+        <v>9.1353150000000003</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="2"/>
-        <v>0.40697687500000002</v>
+        <v>2.5703140625000001</v>
       </c>
       <c r="E10" s="6">
         <f>C5/C10</f>
-        <v>26.001944000668221</v>
+        <v>9.0035264246498343</v>
       </c>
       <c r="F10" s="6">
         <f>B10/B5</f>
@@ -27481,21 +27485,21 @@
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0.81256075002088191</v>
+        <v>0.28136020077030732</v>
       </c>
       <c r="I10" s="4">
         <v>32</v>
       </c>
       <c r="J10" s="5">
-        <v>0.83439416666666599</v>
+        <v>2.6894680000000002</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="3"/>
-        <v>0.40697687500000002</v>
+        <v>2.5703140625000001</v>
       </c>
       <c r="L10" s="6">
         <f>J5/J10</f>
-        <v>15.608042961310264</v>
+        <v>30.58227500754796</v>
       </c>
       <c r="M10" s="6">
         <f>I10/I5</f>
@@ -27503,7 +27507,7 @@
       </c>
       <c r="N10" s="7">
         <f t="shared" si="1"/>
-        <v>0.48775134254094576</v>
+        <v>0.95569609398587374</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27511,15 +27515,15 @@
         <v>64</v>
       </c>
       <c r="C11" s="47">
-        <v>0.46406599999999898</v>
+        <v>1.7077325000000001</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="2"/>
-        <v>0.20348843750000001</v>
+        <v>1.28515703125</v>
       </c>
       <c r="E11" s="10">
         <f>C5/C11</f>
-        <v>28.063378915930123</v>
+        <v>48.163310120291086</v>
       </c>
       <c r="F11" s="10">
         <f>B11/B5</f>
@@ -27527,21 +27531,21 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>0.43849029556140817</v>
+        <v>0.75255172062954823</v>
       </c>
       <c r="I11" s="8">
         <v>64</v>
       </c>
-      <c r="J11" s="9">
-        <v>0.476252333333333</v>
+      <c r="J11" s="47">
+        <v>1.73594</v>
       </c>
       <c r="K11" s="9">
         <f t="shared" si="3"/>
-        <v>0.20348843750000001</v>
+        <v>1.28515703125</v>
       </c>
       <c r="L11" s="10">
         <f>J5/J11</f>
-        <v>27.345293846329383</v>
+        <v>47.380698641658121</v>
       </c>
       <c r="M11" s="10">
         <f>I11/I5</f>
@@ -27549,7 +27553,7 @@
       </c>
       <c r="N11" s="11">
         <f t="shared" si="1"/>
-        <v>0.42727021634889661</v>
+        <v>0.74032341627590814</v>
       </c>
     </row>
   </sheetData>
@@ -27570,8 +27574,8 @@
   </sheetPr>
   <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="G1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27654,11 +27658,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>13.023260000000001</v>
+        <v>82.766475</v>
       </c>
       <c r="D5" s="5">
         <f>C5/B5</f>
-        <v>13.023260000000001</v>
+        <v>82.766475</v>
       </c>
       <c r="E5" s="6">
         <f>C5/C5</f>
@@ -27676,11 +27680,11 @@
         <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>13.023260000000001</v>
+        <v>82.753500000000003</v>
       </c>
       <c r="K5" s="5">
         <f>J5</f>
-        <v>13.023260000000001</v>
+        <v>82.753500000000003</v>
       </c>
       <c r="L5" s="6">
         <f>K5/J5</f>
@@ -27700,15 +27704,15 @@
         <v>2</v>
       </c>
       <c r="C6" s="9">
-        <v>7.8162839999999996</v>
+        <v>52.150500000000001</v>
       </c>
       <c r="D6" s="5">
         <f>C5/B6</f>
-        <v>6.5116300000000003</v>
+        <v>41.3832375</v>
       </c>
       <c r="E6" s="6">
         <f>C5/C6</f>
-        <v>1.6661702670987903</v>
+        <v>1.5870696349987057</v>
       </c>
       <c r="F6" s="6">
         <f>B6/B5</f>
@@ -27716,28 +27720,28 @@
       </c>
       <c r="G6" s="7">
         <f t="shared" ref="G6:G11" si="0">E6/F6</f>
-        <v>0.83308513354939517</v>
+        <v>0.79353481749935284</v>
       </c>
       <c r="I6" s="4">
         <v>2</v>
       </c>
       <c r="J6" s="9">
-        <v>7.7582259999999996</v>
+        <v>51.924399999999999</v>
       </c>
       <c r="K6" s="5">
         <f>K5/I6</f>
-        <v>6.5116300000000003</v>
+        <v>41.376750000000001</v>
       </c>
       <c r="L6" s="6">
         <f>J5/J6</f>
-        <v>1.67863890533738</v>
+        <v>1.5937305004968763</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
       </c>
       <c r="N6" s="7">
         <f>L6/M6</f>
-        <v>0.83931945266869001</v>
+        <v>0.79686525024843813</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27745,15 +27749,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="9">
-        <v>2.9726299999999899</v>
+        <v>21.254525000000001</v>
       </c>
       <c r="D7" s="5">
         <f>C5/B7</f>
-        <v>3.2558150000000001</v>
+        <v>20.69161875</v>
       </c>
       <c r="E7" s="6">
         <f>C5/C7</f>
-        <v>4.3810565055186972</v>
+        <v>3.8940637346635598</v>
       </c>
       <c r="F7" s="6">
         <f>B7/B5</f>
@@ -27761,21 +27765,21 @@
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>1.0952641263796743</v>
+        <v>0.97351593366588995</v>
       </c>
       <c r="I7" s="4">
         <v>4</v>
       </c>
       <c r="J7" s="9">
-        <v>2.9892599999999998</v>
+        <v>21.266279999999998</v>
       </c>
       <c r="K7" s="5">
         <f>K5/I7</f>
-        <v>3.2558150000000001</v>
+        <v>20.688375000000001</v>
       </c>
       <c r="L7" s="6">
         <f>J5/J7</f>
-        <v>4.3566835939329467</v>
+        <v>3.8913011584536652</v>
       </c>
       <c r="M7" s="6">
         <f>I7/I5</f>
@@ -27783,7 +27787,7 @@
       </c>
       <c r="N7" s="7">
         <f t="shared" ref="N7:N12" si="1">L7/M7</f>
-        <v>1.0891708984832367</v>
+        <v>0.9728252896134163</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27791,15 +27795,15 @@
         <v>8</v>
       </c>
       <c r="C8" s="9">
-        <v>1.5325120000000001</v>
+        <v>9.6265000000000001</v>
       </c>
       <c r="D8" s="5">
         <f>C5/B8</f>
-        <v>1.6279075000000001</v>
+        <v>10.345809375</v>
       </c>
       <c r="E8" s="6">
         <f>C5/C8</f>
-        <v>8.4979823975277196</v>
+        <v>8.5977743728250147</v>
       </c>
       <c r="F8" s="6">
         <f>B8/B5</f>
@@ -27807,21 +27811,21 @@
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>1.0622477996909649</v>
+        <v>1.0747217966031268</v>
       </c>
       <c r="I8" s="4">
         <v>8</v>
       </c>
       <c r="J8" s="9">
-        <v>1.538462</v>
+        <v>9.6118299999999994</v>
       </c>
       <c r="K8" s="5">
         <f>K5/I8</f>
-        <v>1.6279075000000001</v>
+        <v>10.3441875</v>
       </c>
       <c r="L8" s="6">
         <f>J5/J8</f>
-        <v>8.4651164604650617</v>
+        <v>8.609546777252616</v>
       </c>
       <c r="M8" s="6">
         <f>I8/I5</f>
@@ -27829,7 +27833,7 @@
       </c>
       <c r="N8" s="7">
         <f t="shared" si="1"/>
-        <v>1.0581395575581327</v>
+        <v>1.076193347156577</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27837,15 +27841,15 @@
         <v>16</v>
       </c>
       <c r="C9" s="9">
-        <v>0.80468039999999996</v>
+        <v>4.7676224999999999</v>
       </c>
       <c r="D9" s="5">
         <f>C5/B9</f>
-        <v>0.81395375000000003</v>
+        <v>5.1729046875</v>
       </c>
       <c r="E9" s="6">
         <f>C5/C9</f>
-        <v>16.184388236621647</v>
+        <v>17.360115025885545</v>
       </c>
       <c r="F9" s="6">
         <f>B9/B5</f>
@@ -27853,21 +27857,21 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>1.0115242647888529</v>
+        <v>1.0850071891178465</v>
       </c>
       <c r="I9" s="4">
         <v>16</v>
       </c>
       <c r="J9" s="9">
-        <v>0.80772960000000005</v>
+        <v>4.7447100000000004</v>
       </c>
       <c r="K9" s="5">
         <f>K5/I9</f>
-        <v>0.81395375000000003</v>
+        <v>5.1720937500000002</v>
       </c>
       <c r="L9" s="6">
         <f>J5/J9</f>
-        <v>16.123291755062585</v>
+        <v>17.441213477746796</v>
       </c>
       <c r="M9" s="6">
         <f>I9/I5</f>
@@ -27875,7 +27879,7 @@
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>1.0077057346914116</v>
+        <v>1.0900758423591748</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27883,15 +27887,15 @@
         <v>32</v>
       </c>
       <c r="C10" s="9">
-        <v>0.41275420000000002</v>
+        <v>2.4055300000000002</v>
       </c>
       <c r="D10" s="5">
         <f>C5/B10</f>
-        <v>0.40697687500000002</v>
+        <v>2.58645234375</v>
       </c>
       <c r="E10" s="6">
         <f>C5/C10</f>
-        <v>31.552095654023631</v>
+        <v>34.406752358108193</v>
       </c>
       <c r="F10" s="6">
         <f>B10/B5</f>
@@ -27899,21 +27903,21 @@
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0.98600298918823848</v>
+        <v>1.075211011190881</v>
       </c>
       <c r="I10" s="4">
         <v>32</v>
       </c>
       <c r="J10" s="9">
-        <v>0.411412</v>
+        <v>2.4048430000000001</v>
       </c>
       <c r="K10" s="5">
         <f>K5/I10</f>
-        <v>0.40697687500000002</v>
+        <v>2.5860468750000001</v>
       </c>
       <c r="L10" s="6">
         <f>J5/J10</f>
-        <v>31.655031938786426</v>
+        <v>34.411186094061023</v>
       </c>
       <c r="M10" s="6">
         <f>I10/I5</f>
@@ -27921,7 +27925,7 @@
       </c>
       <c r="N10" s="7">
         <f t="shared" si="1"/>
-        <v>0.9892197480870758</v>
+        <v>1.075349565439407</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27929,15 +27933,15 @@
         <v>64</v>
       </c>
       <c r="C11" s="9">
-        <v>0.2284128</v>
+        <v>1.3127530000000001</v>
       </c>
       <c r="D11" s="9">
         <f>C5/B11</f>
-        <v>0.20348843750000001</v>
+        <v>1.293226171875</v>
       </c>
       <c r="E11" s="10">
         <f>C5/C11</f>
-        <v>57.016331834292998</v>
+        <v>63.048018172497031</v>
       </c>
       <c r="F11" s="10">
         <f>B11/B5</f>
@@ -27945,21 +27949,21 @@
       </c>
       <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>0.8908801849108281</v>
+        <v>0.98512528394526611</v>
       </c>
       <c r="I11" s="4">
         <v>64</v>
       </c>
       <c r="J11" s="9">
-        <v>0.225692799999999</v>
+        <v>1.3067599999999999</v>
       </c>
       <c r="K11" s="5">
         <f>K5/I11</f>
-        <v>0.20348843750000001</v>
+        <v>1.2930234375</v>
       </c>
       <c r="L11" s="6">
         <f>J5/J11</f>
-        <v>57.703480128741624</v>
+        <v>63.32723683002235</v>
       </c>
       <c r="M11" s="6">
         <f>I11/I5</f>
@@ -27967,7 +27971,7 @@
       </c>
       <c r="N11" s="7">
         <f t="shared" si="1"/>
-        <v>0.90161687701158788</v>
+        <v>0.98948807546909923</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -27975,15 +27979,15 @@
         <v>128</v>
       </c>
       <c r="J12" s="9">
-        <v>0.1447996</v>
+        <v>0.69983574999999998</v>
       </c>
       <c r="K12" s="9">
         <f>K5/I12</f>
-        <v>0.10174421875</v>
+        <v>0.64651171875000002</v>
       </c>
       <c r="L12" s="10">
         <f>J5/J12</f>
-        <v>89.939889336710877</v>
+        <v>118.2470315356139</v>
       </c>
       <c r="M12" s="10">
         <f>I12/I5</f>
@@ -27991,7 +27995,7 @@
       </c>
       <c r="N12" s="11">
         <f t="shared" si="1"/>
-        <v>0.70265538544305373</v>
+        <v>0.92380493387198359</v>
       </c>
     </row>
   </sheetData>
@@ -28012,8 +28016,8 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28112,15 +28116,15 @@
         <v>1</v>
       </c>
       <c r="C4" s="48">
-        <v>13.3470333333333</v>
+        <v>83.885300000000001</v>
       </c>
       <c r="D4" s="5">
         <f>'Strong MPI'!C5/2</f>
-        <v>6.5116300000000003</v>
+        <v>41.3832375</v>
       </c>
       <c r="E4" s="6">
         <f>'Strong MPI'!C5/C4</f>
-        <v>0.97574192517188829</v>
+        <v>0.98666244264489722</v>
       </c>
       <c r="F4" s="6">
         <f>B4*2</f>
@@ -28128,18 +28132,18 @@
       </c>
       <c r="G4" s="22">
         <f t="shared" ref="G4:G9" si="0">E4/F4</f>
-        <v>0.48787096258594415</v>
+        <v>0.49333122132244861</v>
       </c>
       <c r="H4" s="5">
-        <v>13.550233333333299</v>
+        <v>84.641999999999996</v>
       </c>
       <c r="I4" s="5">
         <f>'Strong MPI'!C5/4</f>
-        <v>3.2558150000000001</v>
+        <v>20.69161875</v>
       </c>
       <c r="J4" s="6">
         <f>'Strong MPI'!C5/H4</f>
-        <v>0.96110964878833816</v>
+        <v>0.97784167434606939</v>
       </c>
       <c r="K4" s="6">
         <f>B4*4</f>
@@ -28147,18 +28151,18 @@
       </c>
       <c r="L4" s="22">
         <f>J4/K4</f>
-        <v>0.24027741219708454</v>
+        <v>0.24446041858651735</v>
       </c>
       <c r="M4" s="5">
-        <v>13.9047666666666</v>
+        <v>84.36</v>
       </c>
       <c r="N4" s="5">
         <f>'Strong MPI'!C5/8</f>
-        <v>1.6279075000000001</v>
+        <v>10.345809375</v>
       </c>
       <c r="O4" s="6">
         <f>'Strong MPI'!C5/M4</f>
-        <v>0.93660399431370511</v>
+        <v>0.98111041963015644</v>
       </c>
       <c r="P4" s="6">
         <f>B4*8</f>
@@ -28166,7 +28170,7 @@
       </c>
       <c r="Q4" s="21">
         <f>O4/P4</f>
-        <v>0.11707549928921314</v>
+        <v>0.12263880245376955</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -28175,15 +28179,15 @@
         <v>2</v>
       </c>
       <c r="C5" s="48">
-        <v>7.94969666666666</v>
+        <v>52.741325000000003</v>
       </c>
       <c r="D5" s="5">
         <f>D4/B5</f>
-        <v>3.2558150000000001</v>
+        <v>20.69161875</v>
       </c>
       <c r="E5" s="6">
         <f>'Strong MPI'!C5/C5</f>
-        <v>1.6382084180151122</v>
+        <v>1.5692907790996906</v>
       </c>
       <c r="F5" s="6">
         <f>B5*2</f>
@@ -28191,18 +28195,18 @@
       </c>
       <c r="G5" s="22">
         <f t="shared" si="0"/>
-        <v>0.40955210450377805</v>
-      </c>
-      <c r="H5" s="5">
-        <v>8.0299083333333297</v>
+        <v>0.39232269477492265</v>
+      </c>
+      <c r="H5" s="48">
+        <v>52.741325000000003</v>
       </c>
       <c r="I5" s="5">
         <f>I4/B5</f>
-        <v>1.6279075000000001</v>
+        <v>10.345809375</v>
       </c>
       <c r="J5" s="6">
         <f>'Strong MPI'!C5/H5</f>
-        <v>1.6218441680010884</v>
+        <v>1.5692907790996906</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" ref="K5:K8" si="1">B5*4</f>
@@ -28210,18 +28214,18 @@
       </c>
       <c r="L5" s="22">
         <f>J5/K5</f>
-        <v>0.20273052100013605</v>
+        <v>0.19616134738746133</v>
       </c>
       <c r="M5" s="5">
-        <v>8.3170016666666609</v>
+        <v>52.997</v>
       </c>
       <c r="N5" s="5">
         <f>N4/B5</f>
-        <v>0.81395375000000003</v>
+        <v>5.1729046875</v>
       </c>
       <c r="O5" s="6">
         <f>'Strong MPI'!C5/M5</f>
-        <v>1.5658599723738595</v>
+        <v>1.5617200030190388</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" ref="P5:P7" si="2">B5*8</f>
@@ -28229,7 +28233,7 @@
       </c>
       <c r="Q5" s="22">
         <f>O5/P5</f>
-        <v>9.7866248273366221E-2</v>
+        <v>9.7607500188689925E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -28238,15 +28242,15 @@
         <v>4</v>
       </c>
       <c r="C6" s="48">
-        <v>1.6680979999999901</v>
+        <v>10.39695</v>
       </c>
       <c r="D6" s="5">
         <f>D4/B6</f>
-        <v>1.6279075000000001</v>
+        <v>10.345809375</v>
       </c>
       <c r="E6" s="6">
         <f>'Strong MPI'!C5/C6</f>
-        <v>7.8072511327272602</v>
+        <v>7.960649517406547</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" ref="F6:F8" si="3">B6*2</f>
@@ -28254,18 +28258,18 @@
       </c>
       <c r="G6" s="22">
         <f t="shared" si="0"/>
-        <v>0.97590639159090753</v>
+        <v>0.99508118967581838</v>
       </c>
       <c r="H6" s="5">
-        <v>0.90440083333333299</v>
+        <v>6.44367</v>
       </c>
       <c r="I6" s="5">
         <f>I4/B6</f>
-        <v>0.81395375000000003</v>
+        <v>5.1729046875</v>
       </c>
       <c r="J6" s="6">
         <f>'Strong MPI'!C5/H6</f>
-        <v>14.399876161104826</v>
+        <v>12.844617275558804</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="1"/>
@@ -28273,18 +28277,18 @@
       </c>
       <c r="L6" s="22">
         <f t="shared" ref="L6:L8" si="4">J6/K6</f>
-        <v>0.89999226006905164</v>
+        <v>0.80278857972242523</v>
       </c>
       <c r="M6" s="5">
-        <v>0.53570533333333303</v>
+        <v>6.4591700000000003</v>
       </c>
       <c r="N6" s="5">
         <f>N4/B6</f>
-        <v>0.40697687500000002</v>
+        <v>2.58645234375</v>
       </c>
       <c r="O6" s="6">
         <f>'Strong MPI'!C5/M6</f>
-        <v>24.310491588659453</v>
+        <v>12.813794187178848</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="2"/>
@@ -28292,7 +28296,7 @@
       </c>
       <c r="Q6" s="22">
         <f t="shared" ref="Q6:Q7" si="5">O6/P6</f>
-        <v>0.75970286214560789</v>
+        <v>0.400431068349339</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.4">
@@ -28301,15 +28305,15 @@
         <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>0.92075016666666598</v>
+        <v>5.0351224999999999</v>
       </c>
       <c r="D7" s="5">
         <f>D4/B7</f>
-        <v>0.81395375000000003</v>
+        <v>5.1729046875</v>
       </c>
       <c r="E7" s="6">
         <f>'Strong MPI'!C5/C7</f>
-        <v>14.144184243970644</v>
+        <v>16.437827480860694</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="3"/>
@@ -28317,18 +28321,18 @@
       </c>
       <c r="G7" s="22">
         <f t="shared" si="0"/>
-        <v>0.88401151524816524</v>
+        <v>1.0273642175537934</v>
       </c>
       <c r="H7" s="5">
-        <v>0.50214416666666595</v>
+        <v>2.6307100000000001</v>
       </c>
       <c r="I7" s="5">
         <f>I4/B7</f>
-        <v>0.40697687500000002</v>
+        <v>2.58645234375</v>
       </c>
       <c r="J7" s="6">
         <f>'Strong MPI'!C5/H7</f>
-        <v>25.935300785133126</v>
+        <v>31.461649136544885</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="1"/>
@@ -28336,18 +28340,18 @@
       </c>
       <c r="L7" s="22">
         <f t="shared" si="4"/>
-        <v>0.8104781495354102</v>
+        <v>0.98317653551702766</v>
       </c>
       <c r="M7" s="5">
-        <v>0.302153</v>
+        <v>1.51515</v>
       </c>
       <c r="N7" s="5">
         <f>N4/B7</f>
-        <v>0.20348843750000001</v>
+        <v>1.293226171875</v>
       </c>
       <c r="O7" s="6">
         <f>'Strong MPI'!C5/M7</f>
-        <v>43.101541272136963</v>
+        <v>54.625928125928127</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
@@ -28355,7 +28359,7 @@
       </c>
       <c r="Q7" s="22">
         <f t="shared" si="5"/>
-        <v>0.67346158237714004</v>
+        <v>0.85353012696762698</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.4">
@@ -28364,15 +28368,15 @@
         <v>16</v>
       </c>
       <c r="C8" s="49">
-        <v>41.6880666666666</v>
+        <v>49.744900000000001</v>
       </c>
       <c r="D8" s="5">
         <f>D4/B8</f>
-        <v>0.40697687500000002</v>
+        <v>2.58645234375</v>
       </c>
       <c r="E8" s="6">
         <f>'Strong MPI'!C5/C8</f>
-        <v>0.31239779249377569</v>
+        <v>1.6638183009715568</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="3"/>
@@ -28380,18 +28384,18 @@
       </c>
       <c r="G8" s="22">
         <f t="shared" si="0"/>
-        <v>9.7624310154304905E-3</v>
+        <v>5.199432190536115E-2</v>
       </c>
       <c r="H8" s="5">
-        <v>37.889233333333301</v>
+        <v>47.2241</v>
       </c>
       <c r="I8" s="5">
         <f>I4/B8</f>
-        <v>0.20348843750000001</v>
+        <v>1.293226171875</v>
       </c>
       <c r="J8" s="6">
         <f>'Strong MPI'!C5/H8</f>
-        <v>0.34371927997135543</v>
+        <v>1.7526321306282173</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="1"/>
@@ -28399,7 +28403,7 @@
       </c>
       <c r="L8" s="22">
         <f t="shared" si="4"/>
-        <v>5.3706137495524286E-3</v>
+        <v>2.7384877041065896E-2</v>
       </c>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
@@ -28413,15 +28417,15 @@
         <v>32</v>
       </c>
       <c r="C9" s="8">
-        <v>75.660216666666599</v>
+        <v>94.252200000000002</v>
       </c>
       <c r="D9" s="9">
         <f>D4/B9</f>
-        <v>0.20348843750000001</v>
+        <v>1.293226171875</v>
       </c>
       <c r="E9" s="10">
         <f>'Strong MPI'!C5/C9</f>
-        <v>0.17212824088749432</v>
+        <v>0.8781383882816528</v>
       </c>
       <c r="F9" s="10">
         <f>B9*2</f>
@@ -28429,7 +28433,7 @@
       </c>
       <c r="G9" s="23">
         <f t="shared" si="0"/>
-        <v>2.6895037638670987E-3</v>
+        <v>1.3720912316900825E-2</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -28461,7 +28465,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update excel avec weak
</commit_message>
<xml_diff>
--- a/Analyse .out/ScalabilityShallow.xlsx
+++ b/Analyse .out/ScalabilityShallow.xlsx
@@ -1,47 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9be20e56d8dc8fd/Documents/GitHub/Projet-HPC/Analyse .out/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colli\OneDrive - Universite de Liege\Documents\Projet HPC\Projet-HPC\Analyse .out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{07A788C6-E1AB-4A6F-A8A8-DB69971995BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D03B1CDE-7AA6-4BD1-950C-8918676FF935}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840D2E5-2AB1-4F14-91D5-435A1E9F3742}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="2" xr2:uid="{F37CA3FF-E8FD-40D0-995D-F29E9880726D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22620" windowHeight="13500" firstSheet="4" activeTab="5" xr2:uid="{F37CA3FF-E8FD-40D0-995D-F29E9880726D}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong OpenMP" sheetId="4" r:id="rId1"/>
     <sheet name="Strong MPI" sheetId="1" r:id="rId2"/>
     <sheet name="Strong Hybrid" sheetId="6" r:id="rId3"/>
     <sheet name="Weak OpenMP" sheetId="7" r:id="rId4"/>
-    <sheet name="Weak MPI" sheetId="8" r:id="rId5"/>
-    <sheet name="Weak Hybrid" sheetId="9" r:id="rId6"/>
+    <sheet name="Weak MPI (2)" sheetId="10" r:id="rId5"/>
+    <sheet name="Weak Hybrid (2)" sheetId="11" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
   <si>
     <t>Speedup</t>
   </si>
@@ -96,6 +88,9 @@
   <si>
     <t>Bind spread</t>
   </si>
+  <si>
+    <t>Num ranks</t>
+  </si>
 </sst>
 </file>
 
@@ -104,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -468,12 +463,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +545,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -978,7 +967,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1013,7 +1002,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -1098,7 +1087,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1133,7 +1122,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -1196,7 +1185,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1231,7 +1220,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
@@ -1287,7 +1276,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1328,7 +1317,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1402,7 +1391,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1677,7 +1666,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1712,7 +1701,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -1724,7 +1713,6 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1787,7 +1775,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1822,7 +1810,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -1861,7 +1849,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1902,7 +1890,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1977,7 +1965,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2374,7 +2362,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2409,7 +2397,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -2494,7 +2482,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2529,7 +2517,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -2542,8 +2530,6 @@
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -2592,7 +2578,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2627,14 +2613,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -2683,7 +2667,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2724,7 +2708,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2795,7 +2779,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3201,7 +3185,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3236,7 +3220,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -3321,7 +3305,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3356,7 +3340,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -3369,8 +3353,6 @@
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -3419,7 +3401,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3454,14 +3436,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -3510,7 +3490,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3551,7 +3531,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3625,7 +3605,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3894,7 +3874,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3929,7 +3909,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -3941,7 +3921,6 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4004,7 +3983,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4039,7 +4018,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -4078,7 +4057,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4119,7 +4098,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4193,7 +4172,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4456,7 +4435,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4491,7 +4470,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -4503,7 +4482,6 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4566,7 +4544,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4601,7 +4579,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -4640,7 +4618,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4681,7 +4659,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4756,7 +4734,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4852,25 +4830,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>229.983</c:v>
+                  <c:v>13.195</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>306.70800000000003</c:v>
+                  <c:v>30.727219999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>365.62700000000001</c:v>
+                  <c:v>48.138280000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>381.53899999999999</c:v>
+                  <c:v>92.040300000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>414.339</c:v>
+                  <c:v>167.1386</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>445.15</c:v>
+                  <c:v>254.89240000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>512.91600000000005</c:v>
+                  <c:v>496.21600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4966,22 +4944,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74984349935443484</c:v>
+                  <c:v>0.42942381380417755</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62900989259545925</c:v>
+                  <c:v>0.27410617911566426</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60277717349995674</c:v>
+                  <c:v>0.14336111464217305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55505998711200255</c:v>
+                  <c:v>7.8946455217406397E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51664158148938566</c:v>
+                  <c:v>5.1766941658519437E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44838336101817838</c:v>
+                  <c:v>2.659124252341722E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5073,7 +5051,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5108,7 +5086,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -5120,7 +5098,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5191,7 +5168,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5226,20 +5203,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.2"/>
-          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -5296,7 +5270,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5331,14 +5305,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -5388,7 +5360,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5429,7 +5401,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5504,7 +5476,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5600,25 +5572,25 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>230.27500000000001</c:v>
+                  <c:v>13.228260000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>226.72300000000001</c:v>
+                  <c:v>17.96048</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>248.25399999999999</c:v>
+                  <c:v>26.319099999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>260.38600000000002</c:v>
+                  <c:v>58.044020000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>309.44499999999999</c:v>
+                  <c:v>107.8432</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>359.53100000000001</c:v>
+                  <c:v>226.42859999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>528.96699999999998</c:v>
+                  <c:v>495.38279999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5714,22 +5686,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0156666946009005</c:v>
+                  <c:v>0.73652040479987169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92757820619204534</c:v>
+                  <c:v>0.50261065158003126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88436014225035131</c:v>
+                  <c:v>0.22790047967042945</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74415485789073987</c:v>
+                  <c:v>0.12266197590575949</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64048719025619483</c:v>
+                  <c:v>5.8421330167655508E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43532961413471921</c:v>
+                  <c:v>2.670310717287722E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5821,7 +5793,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5856,7 +5828,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -5868,7 +5840,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5939,7 +5910,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5974,20 +5945,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.2"/>
-          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -6044,7 +6012,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6079,14 +6047,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -6136,7 +6102,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6177,7 +6143,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6252,7 +6218,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6275,9 +6241,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Execution time</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="38100" cap="rnd">
               <a:solidFill>
@@ -6313,10 +6276,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$B$4:$B$11</c:f>
+              <c:f>'Weak MPI (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6337,42 +6300,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$C$4:$C$11</c:f>
+              <c:f>'Weak MPI (2)'!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>230.39099999999999</c:v>
+                  <c:v>13.062200000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>227.08199999999999</c:v>
+                  <c:v>17.616099999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>228.239</c:v>
+                  <c:v>12.9846</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>227.19499999999999</c:v>
+                  <c:v>13.7319</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>234.80600000000001</c:v>
+                  <c:v>15.492599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>236.06899999999999</c:v>
+                  <c:v>26.883199999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>241.56100000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>248.33699999999999</c:v>
+                  <c:v>54.066200000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6380,7 +6337,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F6E4-422F-BFED-4DF99705FDDC}"/>
+              <c16:uniqueId val="{00000000-35CB-4645-9FA3-A782D2F8EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6401,9 +6358,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Weak scaling efficiency</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="38100" cap="rnd">
               <a:solidFill>
@@ -6430,10 +6384,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$B$4:$B$11</c:f>
+              <c:f>'Weak MPI (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6454,42 +6408,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$D$4:$D$11</c:f>
+              <c:f>'Weak MPI (2)'!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0145718286786272</c:v>
+                  <c:v>0.74149215774206556</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0094287128843011</c:v>
+                  <c:v>1.005976310398472</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0140672109861573</c:v>
+                  <c:v>0.95123034685658947</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98119724368201822</c:v>
+                  <c:v>0.84312510488878567</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97594771020337279</c:v>
+                  <c:v>0.48588709677419362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95375909190639208</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.92773529518356102</c:v>
+                  <c:v>0.24159641328593465</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6497,7 +6445,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F6E4-422F-BFED-4DF99705FDDC}"/>
+              <c16:uniqueId val="{00000001-35CB-4645-9FA3-A782D2F8EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6554,7 +6502,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-BE" b="1"/>
-                  <a:t>Number of threads</a:t>
+                  <a:t>Number of ranks</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6581,7 +6529,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6616,7 +6564,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -6628,8 +6576,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="250"/>
-          <c:min val="210"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6700,7 +6646,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6735,20 +6681,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -6805,7 +6748,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6840,13 +6783,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -6896,7 +6838,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6937,7 +6879,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6984,7 +6926,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-BE" sz="1600" b="1" baseline="0"/>
-              <a:t> MPI Weak Scaling (close) </a:t>
+              <a:t> Hybid Weak Scaling (2 threads) </a:t>
             </a:r>
             <a:endParaRPr lang="fr-BE" sz="1600" b="1"/>
           </a:p>
@@ -7012,7 +6954,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7073,10 +7015,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$B$4:$B$11</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -7097,42 +7039,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$E$4:$E$11</c:f>
+              <c:f>'Weak Hybrid (2)'!$C$4:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>230.63399999999999</c:v>
+                  <c:v>27.9283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>226.55</c:v>
+                  <c:v>34.0608</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>228.81</c:v>
+                  <c:v>34.138300000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>226.61</c:v>
+                  <c:v>32.020699999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>227.22399999999999</c:v>
+                  <c:v>54.841900000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>231.97499999999999</c:v>
+                  <c:v>67.715400000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>237.21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>247.124</c:v>
+                  <c:v>174.32409999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7140,7 +7076,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-00FF-4064-AE62-78EC3B520D6B}"/>
+              <c16:uniqueId val="{00000000-6C50-4C07-A4F9-D938A91BD7D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7190,10 +7126,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$B$4:$B$11</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -7214,42 +7150,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak MPI'!$F$4:$F$11</c:f>
+              <c:f>'Weak Hybrid (2)'!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0180269256234826</c:v>
+                  <c:v>0.81995431698609544</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0079716795594598</c:v>
+                  <c:v>0.81809287515781393</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0177573805216009</c:v>
+                  <c:v>0.87219517374698252</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0150072175474421</c:v>
+                  <c:v>0.50925113827201463</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99421920465567404</c:v>
+                  <c:v>0.41243646201602591</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.97227772859491579</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.93327236529029955</c:v>
+                  <c:v>0.16020905887367268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7257,7 +7187,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-00FF-4064-AE62-78EC3B520D6B}"/>
+              <c16:uniqueId val="{00000001-6C50-4C07-A4F9-D938A91BD7D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7277,7 +7207,7 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="128"/>
+          <c:max val="64"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7314,8 +7244,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-BE" b="1"/>
-                  <a:t>Number of threads</a:t>
+                  <a:t>Number of</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" b="1" baseline="0"/>
+                  <a:t> ranks</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-BE" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -7341,7 +7276,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7376,7 +7311,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -7388,8 +7323,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="250"/>
-          <c:min val="210"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7460,7 +7393,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7495,20 +7428,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -7565,7 +7495,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7600,13 +7530,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -7656,7 +7585,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7697,7 +7626,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7744,7 +7673,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-BE" sz="1600" b="1" baseline="0"/>
-              <a:t> Hybid Weak Scaling (2 threads) </a:t>
+              <a:t> Hybid Weak Scaling (4 threads) </a:t>
             </a:r>
             <a:endParaRPr lang="fr-BE" sz="1600" b="1"/>
           </a:p>
@@ -7772,7 +7701,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7833,7 +7762,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$B$4:$B$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7863,30 +7792,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$C$4:$C$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$E$4:$E$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>226.73099999999999</c:v>
+                  <c:v>54.374299999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>227.59899999999999</c:v>
+                  <c:v>67.715400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227.459</c:v>
+                  <c:v>109.3655</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>235.167</c:v>
+                  <c:v>110.8036</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>234.31200000000001</c:v>
+                  <c:v>219.17310000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>238.76300000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>241.352</c:v>
+                  <c:v>399.65940000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7894,7 +7820,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2F30-4829-A286-B79EB14A178C}"/>
+              <c16:uniqueId val="{00000000-610B-411D-89A2-D17034E1C000}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7944,7 +7870,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$B$4:$B$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7974,30 +7900,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$D$4:$D$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$F$4:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99618627498363355</c:v>
+                  <c:v>0.80298277792053208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99679942319275117</c:v>
+                  <c:v>0.49717964074593907</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96412761994667617</c:v>
+                  <c:v>0.49072683559017932</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96764570316501064</c:v>
+                  <c:v>0.24808838310905854</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94960693239739824</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.93942043156882893</c:v>
+                  <c:v>0.1360515979356422</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8005,7 +7928,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2F30-4829-A286-B79EB14A178C}"/>
+              <c16:uniqueId val="{00000001-610B-411D-89A2-D17034E1C000}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8025,7 +7948,7 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="64"/>
+          <c:max val="32"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8062,7 +7985,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-BE" b="1"/>
-                  <a:t>Number of threads</a:t>
+                  <a:t>Number of ranks</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8089,7 +8012,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8124,7 +8047,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -8136,8 +8059,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="250"/>
-          <c:min val="210"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8208,7 +8129,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8243,20 +8164,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -8313,7 +8231,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8348,13 +8266,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -8404,7 +8321,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8445,7 +8362,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8523,7 +8440,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8820,7 +8737,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8855,7 +8772,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -8928,7 +8845,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8963,7 +8880,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -9002,7 +8919,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9043,7 +8960,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9067,6 +8984,7 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -9090,12 +9008,20 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-BE" sz="1600" b="1" baseline="0"/>
-              <a:t> Hybid Weak Scaling (4 threads) </a:t>
+              <a:t> Hybid Weak Scaling (8 threads) </a:t>
             </a:r>
             <a:endParaRPr lang="fr-BE" sz="1600" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18156879669437778"/>
+          <c:y val="1.390101274898E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9118,7 +9044,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9145,12 +9071,9 @@
             <c:v>Execution time</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9179,7 +9102,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$B$4:$B$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -9209,27 +9132,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$E$4:$E$9</c:f>
+              <c:f>'Weak Hybrid (2)'!$G$4:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>247.55099999999999</c:v>
+                  <c:v>109.9502</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>231.38200000000001</c:v>
+                  <c:v>132.13669999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>234.047</c:v>
+                  <c:v>435.66809999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>237.614</c:v>
+                  <c:v>440.1814</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>242.185</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>241.512</c:v>
+                  <c:v>874.27629999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9237,7 +9157,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2668-4C07-ABB8-123AD204167F}"/>
+              <c16:uniqueId val="{00000000-7319-4646-98A1-90B8CEB626CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9262,9 +9182,9 @@
             <c:v>Weak scaling efficiency</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -9287,7 +9207,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$B$4:$B$10</c:f>
+              <c:f>'Weak Hybrid (2)'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -9317,27 +9237,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Weak Hybrid'!$F$4:$F$9</c:f>
+              <c:f>'Weak Hybrid (2)'!$H$4:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0698801116767942</c:v>
+                  <c:v>0.83209433866594218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0576978128324652</c:v>
+                  <c:v>0.25237147268758031</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.041819926435311</c:v>
+                  <c:v>0.24978383911723664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0221566158102278</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0250049686972076</c:v>
+                  <c:v>0.12576138687506455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9345,7 +9262,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2668-4C07-ABB8-123AD204167F}"/>
+              <c16:uniqueId val="{00000001-7319-4646-98A1-90B8CEB626CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9402,7 +9319,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-BE" b="1"/>
-                  <a:t>Number of threads</a:t>
+                  <a:t>Number of ranks</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9429,7 +9346,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9464,7 +9381,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -9476,8 +9393,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="250"/>
-          <c:min val="210"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -9548,7 +9463,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9583,20 +9498,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -9653,7 +9565,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9688,13 +9600,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -9744,7 +9655,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9785,7 +9696,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9856,7 +9767,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10278,7 +10189,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10313,7 +10224,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -10398,7 +10309,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10433,7 +10344,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -10496,7 +10407,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10531,7 +10442,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
@@ -10587,7 +10498,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10628,7 +10539,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10706,7 +10617,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10993,7 +10904,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11028,7 +10939,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -11101,7 +11012,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11136,7 +11047,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -11175,7 +11086,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11216,7 +11127,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11286,7 +11197,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11573,7 +11484,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11608,7 +11519,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -11682,7 +11593,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11717,7 +11628,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -11756,7 +11667,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11797,7 +11708,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11868,7 +11779,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12292,7 +12203,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12327,7 +12238,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -12412,7 +12323,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12447,7 +12358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -12460,8 +12371,6 @@
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1000000000000001"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -12510,7 +12419,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12545,14 +12454,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -12601,7 +12508,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12642,7 +12549,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12713,7 +12620,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13155,7 +13062,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13190,7 +13097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -13275,7 +13182,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13310,7 +13217,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
@@ -13323,7 +13230,6 @@
         <c:axId val="486779375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -13372,7 +13278,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13407,14 +13313,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.2"/>
-        <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486780815"/>
@@ -13463,7 +13367,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13504,7 +13408,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13574,7 +13478,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13873,7 +13777,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13908,7 +13812,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270543679"/>
@@ -13982,7 +13886,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14017,7 +13921,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270548959"/>
@@ -14056,7 +13960,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14097,7 +14001,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14172,7 +14076,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -14560,7 +14464,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14595,7 +14499,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="484399263"/>
@@ -14607,8 +14511,6 @@
         <c:axId val="484399263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="64"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -14679,7 +14581,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14714,14 +14616,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486791855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="8"/>
-        <c:minorUnit val="4"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="486779375"/>
@@ -14776,7 +14676,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14811,7 +14711,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="486780815"/>
@@ -14867,7 +14767,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14908,7 +14808,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -26687,7 +26587,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4720B79-F94C-4946-90BF-BB0941948287}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC2A51F-20D8-4445-BA0B-DF8C2C9EC097}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26702,44 +26602,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA76E4AF-B56B-428B-A6E3-D2D856E0569E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -26765,10 +26627,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="2" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B282362-5796-4D14-AB60-80090DD17E97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2CED15E-B640-42C4-8B26-BEEFBD0B6812}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26803,10 +26665,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="3" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6F5DC3-ED6D-4B34-A9C0-CE97256402CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A634ABF-E933-495A-A64B-26AD1F089BE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26826,7 +26688,290 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>633470</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1105956</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>156554</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0CD32A8-4BB6-4F91-800E-B60EB0E4EE7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Strong OpenMP"/>
+      <sheetName val="Strong MPI"/>
+      <sheetName val="Strong Hybrid"/>
+      <sheetName val="Weak OpenMP"/>
+      <sheetName val="Weak MPI"/>
+      <sheetName val="Weak Hybrid"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4">
+        <row r="4">
+          <cell r="B4">
+            <v>1</v>
+          </cell>
+          <cell r="C4">
+            <v>13.062200000000001</v>
+          </cell>
+          <cell r="D4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>2</v>
+          </cell>
+          <cell r="C5">
+            <v>17.616099999999999</v>
+          </cell>
+          <cell r="D5">
+            <v>0.74149215774206556</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>4</v>
+          </cell>
+          <cell r="C6">
+            <v>12.9846</v>
+          </cell>
+          <cell r="D6">
+            <v>1.005976310398472</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>8</v>
+          </cell>
+          <cell r="C7">
+            <v>13.7319</v>
+          </cell>
+          <cell r="D7">
+            <v>0.95123034685658947</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>16</v>
+          </cell>
+          <cell r="C8">
+            <v>15.492599999999999</v>
+          </cell>
+          <cell r="D8">
+            <v>0.84312510488878567</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>32</v>
+          </cell>
+          <cell r="C9">
+            <v>26.883199999999999</v>
+          </cell>
+          <cell r="D9">
+            <v>0.48588709677419362</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>64</v>
+          </cell>
+          <cell r="C10">
+            <v>54.066200000000002</v>
+          </cell>
+          <cell r="D10">
+            <v>0.24159641328593465</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="4">
+          <cell r="B4">
+            <v>1</v>
+          </cell>
+          <cell r="C4">
+            <v>27.9283</v>
+          </cell>
+          <cell r="D4">
+            <v>1</v>
+          </cell>
+          <cell r="E4">
+            <v>54.374299999999998</v>
+          </cell>
+          <cell r="F4">
+            <v>1</v>
+          </cell>
+          <cell r="G4">
+            <v>109.9502</v>
+          </cell>
+          <cell r="H4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>2</v>
+          </cell>
+          <cell r="C5">
+            <v>34.0608</v>
+          </cell>
+          <cell r="D5">
+            <v>0.81995431698609544</v>
+          </cell>
+          <cell r="E5">
+            <v>67.715400000000002</v>
+          </cell>
+          <cell r="F5">
+            <v>0.80298277792053208</v>
+          </cell>
+          <cell r="G5">
+            <v>132.13669999999999</v>
+          </cell>
+          <cell r="H5">
+            <v>0.83209433866594218</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>4</v>
+          </cell>
+          <cell r="C6">
+            <v>34.138300000000001</v>
+          </cell>
+          <cell r="D6">
+            <v>0.81809287515781393</v>
+          </cell>
+          <cell r="E6">
+            <v>109.3655</v>
+          </cell>
+          <cell r="F6">
+            <v>0.49717964074593907</v>
+          </cell>
+          <cell r="G6">
+            <v>435.66809999999998</v>
+          </cell>
+          <cell r="H6">
+            <v>0.25237147268758031</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>8</v>
+          </cell>
+          <cell r="C7">
+            <v>32.020699999999998</v>
+          </cell>
+          <cell r="D7">
+            <v>0.87219517374698252</v>
+          </cell>
+          <cell r="E7">
+            <v>110.8036</v>
+          </cell>
+          <cell r="F7">
+            <v>0.49072683559017932</v>
+          </cell>
+          <cell r="G7">
+            <v>440.1814</v>
+          </cell>
+          <cell r="H7">
+            <v>0.24978383911723664</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>16</v>
+          </cell>
+          <cell r="C8">
+            <v>54.841900000000003</v>
+          </cell>
+          <cell r="D8">
+            <v>0.50925113827201463</v>
+          </cell>
+          <cell r="E8">
+            <v>219.17310000000001</v>
+          </cell>
+          <cell r="F8">
+            <v>0.24808838310905854</v>
+          </cell>
+          <cell r="G8">
+            <v>874.27629999999999</v>
+          </cell>
+          <cell r="H8">
+            <v>0.12576138687506455</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>32</v>
+          </cell>
+          <cell r="C9">
+            <v>67.715400000000002</v>
+          </cell>
+          <cell r="D9">
+            <v>0.41243646201602591</v>
+          </cell>
+          <cell r="E9">
+            <v>399.65940000000001</v>
+          </cell>
+          <cell r="F9">
+            <v>0.1360515979356422</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>64</v>
+          </cell>
+          <cell r="C10">
+            <v>174.32409999999999</v>
+          </cell>
+          <cell r="D10">
+            <v>0.16020905887367268</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27148,6 +27293,292 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="0E2841"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E8E8E8"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="156082"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="E97132"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="196B24"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="0F9ED5"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="A02B93"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="4EA72E"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="467886"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="96607D"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7315675C-B625-4647-ABCD-7A950D25B2EB}">
   <sheetPr>
@@ -27155,19 +27586,19 @@
   </sheetPr>
   <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A7" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="4" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="16.81640625" customWidth="1"/>
-    <col min="9" max="14" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="4" width="16.796875" style="3" customWidth="1"/>
+    <col min="5" max="7" width="16.796875" customWidth="1"/>
+    <col min="9" max="14" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="30" customHeight="1">
       <c r="B2" s="50" t="s">
         <v>16</v>
       </c>
@@ -27185,7 +27616,7 @@
       <c r="M2" s="50"/>
       <c r="N2" s="50"/>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" ht="14.4" thickBot="1">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -27196,7 +27627,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:14" ht="45" customHeight="1" thickBot="1">
       <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
@@ -27234,7 +27665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" ht="15">
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -27280,7 +27711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" ht="15">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -27326,7 +27757,7 @@
         <v>0.7665671605624037</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:14" ht="15">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -27372,7 +27803,7 @@
         <v>0.48096069281687837</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:14" ht="15">
       <c r="B8" s="4">
         <v>8</v>
       </c>
@@ -27418,7 +27849,7 @@
         <v>0.65862762425913446</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="15">
       <c r="B9" s="4">
         <v>16</v>
       </c>
@@ -27464,7 +27895,7 @@
         <v>0.90966536279533972</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:14" ht="15">
       <c r="B10" s="4">
         <v>32</v>
       </c>
@@ -27510,7 +27941,7 @@
         <v>0.95569609398587374</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" ht="15.6" thickBot="1">
       <c r="B11" s="8">
         <v>64</v>
       </c>
@@ -27574,19 +28005,19 @@
   </sheetPr>
   <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="4" width="16.81640625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="16.81640625" customWidth="1"/>
-    <col min="9" max="14" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="4" width="16.796875" style="3" customWidth="1"/>
+    <col min="5" max="7" width="16.796875" customWidth="1"/>
+    <col min="9" max="14" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" ht="30" customHeight="1">
       <c r="B2" s="50" t="s">
         <v>14</v>
       </c>
@@ -27604,7 +28035,7 @@
       <c r="M2" s="50"/>
       <c r="N2" s="50"/>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" ht="14.4" thickBot="1">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -27615,7 +28046,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="2:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:14" ht="45" customHeight="1" thickBot="1">
       <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
@@ -27653,7 +28084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" ht="15">
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -27699,7 +28130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:14" ht="15.6" thickBot="1">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -27744,7 +28175,7 @@
         <v>0.79686525024843813</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:14" ht="15.6" thickBot="1">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -27790,7 +28221,7 @@
         <v>0.9728252896134163</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:14" ht="15.6" thickBot="1">
       <c r="B8" s="4">
         <v>8</v>
       </c>
@@ -27836,7 +28267,7 @@
         <v>1.076193347156577</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:14" ht="15.6" thickBot="1">
       <c r="B9" s="4">
         <v>16</v>
       </c>
@@ -27882,7 +28313,7 @@
         <v>1.0900758423591748</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:14" ht="15.6" thickBot="1">
       <c r="B10" s="4">
         <v>32</v>
       </c>
@@ -27928,7 +28359,7 @@
         <v>1.075349565439407</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" ht="15.6" thickBot="1">
       <c r="B11" s="8">
         <v>64</v>
       </c>
@@ -27974,7 +28405,7 @@
         <v>0.98948807546909923</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:14" ht="15.6" thickBot="1">
       <c r="I12" s="8">
         <v>128</v>
       </c>
@@ -28016,26 +28447,26 @@
   </sheetPr>
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="12" width="15.81640625" customWidth="1"/>
-    <col min="13" max="14" width="15.81640625" style="3" customWidth="1"/>
-    <col min="15" max="17" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="12" width="15.796875" customWidth="1"/>
+    <col min="13" max="14" width="15.796875" style="3" customWidth="1"/>
+    <col min="15" max="17" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="14.4" thickBot="1">
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="30" customHeight="1" thickBot="1">
       <c r="B2" s="20"/>
       <c r="C2" s="51" t="s">
         <v>8</v>
@@ -28059,7 +28490,7 @@
       <c r="P2" s="58"/>
       <c r="Q2" s="59"/>
     </row>
-    <row r="3" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
         <v>7</v>
@@ -28110,7 +28541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" ht="15.6" thickBot="1">
       <c r="A4" s="24"/>
       <c r="B4" s="4">
         <v>1</v>
@@ -28173,7 +28604,7 @@
         <v>0.12263880245376955</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" ht="15.6" thickBot="1">
       <c r="A5" s="24"/>
       <c r="B5" s="4">
         <v>2</v>
@@ -28236,7 +28667,7 @@
         <v>9.7607500188689925E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" ht="15.6" thickBot="1">
       <c r="A6" s="24"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -28299,7 +28730,7 @@
         <v>0.400431068349339</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="24"/>
       <c r="B7" s="17">
         <v>8</v>
@@ -28362,7 +28793,7 @@
         <v>0.85353012696762698</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="24"/>
       <c r="B8" s="4">
         <v>16</v>
@@ -28411,7 +28842,7 @@
       <c r="P8" s="32"/>
       <c r="Q8" s="33"/>
     </row>
-    <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" ht="15.6" thickBot="1">
       <c r="A9" s="24"/>
       <c r="B9" s="18">
         <v>32</v>
@@ -28463,26 +28894,26 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="2" max="4" width="16.796875" customWidth="1"/>
+    <col min="5" max="5" width="16.796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="14.4" thickBot="1">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1">
       <c r="B2" s="20"/>
       <c r="C2" s="51" t="s">
         <v>13</v>
@@ -28493,7 +28924,7 @@
       </c>
       <c r="F2" s="59"/>
     </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
         <v>5</v>
@@ -28511,150 +28942,326 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="24"/>
       <c r="B4" s="17">
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>229.983</v>
+        <v>13.195</v>
       </c>
       <c r="D4" s="22">
         <f>C4/C4</f>
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>230.27500000000001</v>
+        <v>13.228260000000001</v>
       </c>
       <c r="F4" s="22">
         <f>E4/E4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="24"/>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="5">
-        <v>306.70800000000003</v>
+        <v>30.727219999999999</v>
       </c>
       <c r="D5" s="22">
         <f>C4/C5</f>
-        <v>0.74984349935443484</v>
+        <v>0.42942381380417755</v>
       </c>
       <c r="E5" s="5">
-        <v>226.72300000000001</v>
+        <v>17.96048</v>
       </c>
       <c r="F5" s="22">
         <f>E4/E5</f>
-        <v>1.0156666946009005</v>
+        <v>0.73652040479987169</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="24"/>
       <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>365.62700000000001</v>
+        <v>48.138280000000002</v>
       </c>
       <c r="D6" s="22">
         <f>C4/C6</f>
-        <v>0.62900989259545925</v>
+        <v>0.27410617911566426</v>
       </c>
       <c r="E6" s="5">
-        <v>248.25399999999999</v>
+        <v>26.319099999999999</v>
       </c>
       <c r="F6" s="22">
         <f>E4/E6</f>
-        <v>0.92757820619204534</v>
+        <v>0.50261065158003126</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="24"/>
       <c r="B7" s="17">
         <v>8</v>
       </c>
       <c r="C7" s="5">
-        <v>381.53899999999999</v>
+        <v>92.040300000000002</v>
       </c>
       <c r="D7" s="22">
         <f>C4/C7</f>
-        <v>0.60277717349995674</v>
+        <v>0.14336111464217305</v>
       </c>
       <c r="E7" s="5">
-        <v>260.38600000000002</v>
+        <v>58.044020000000003</v>
       </c>
       <c r="F7" s="22">
         <f>E4/E7</f>
-        <v>0.88436014225035131</v>
+        <v>0.22790047967042945</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="24"/>
       <c r="B8" s="17">
         <v>16</v>
       </c>
       <c r="C8" s="5">
-        <v>414.339</v>
+        <v>167.1386</v>
       </c>
       <c r="D8" s="22">
         <f>C4/C8</f>
-        <v>0.55505998711200255</v>
+        <v>7.8946455217406397E-2</v>
       </c>
       <c r="E8" s="5">
-        <v>309.44499999999999</v>
+        <v>107.8432</v>
       </c>
       <c r="F8" s="22">
         <f>E4/E8</f>
-        <v>0.74415485789073987</v>
+        <v>0.12266197590575949</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="24"/>
       <c r="B9" s="17">
         <v>32</v>
       </c>
       <c r="C9" s="5">
-        <v>445.15</v>
+        <v>254.89240000000001</v>
       </c>
       <c r="D9" s="22">
         <f>C4/C9</f>
-        <v>0.51664158148938566</v>
+        <v>5.1766941658519437E-2</v>
       </c>
       <c r="E9" s="5">
-        <v>359.53100000000001</v>
+        <v>226.42859999999999</v>
       </c>
       <c r="F9" s="22">
         <f>E4/E9</f>
-        <v>0.64048719025619483</v>
+        <v>5.8421330167655508E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="15.6" thickBot="1">
       <c r="A10" s="24"/>
       <c r="B10" s="18">
         <v>64</v>
       </c>
       <c r="C10" s="9">
-        <v>512.91600000000005</v>
+        <v>496.21600000000001</v>
       </c>
       <c r="D10" s="23">
         <f>C4/C10</f>
-        <v>0.44838336101817838</v>
+        <v>2.659124252341722E-2</v>
       </c>
       <c r="E10" s="9">
-        <v>528.96699999999998</v>
+        <v>495.38279999999997</v>
       </c>
       <c r="F10" s="23">
         <f>E4/E10</f>
-        <v>0.43532961413471921</v>
+        <v>2.670310717287722E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7" ht="14.4" thickBot="1">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="2:7" ht="18" thickBot="1">
+      <c r="C49" s="20"/>
+      <c r="D49" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="53"/>
+      <c r="F49" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="59"/>
+    </row>
+    <row r="50" spans="2:7" ht="63" thickBot="1">
+      <c r="B50" s="24"/>
+      <c r="C50" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="15">
+      <c r="B51" s="24"/>
+      <c r="C51" s="17">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>53.816000000000003</v>
+      </c>
+      <c r="E51" s="22">
+        <f>D51/D51</f>
+        <v>1</v>
+      </c>
+      <c r="F51" s="5">
+        <v>53.811999999999998</v>
+      </c>
+      <c r="G51" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="15">
+      <c r="B52" s="24"/>
+      <c r="C52" s="17">
+        <v>2</v>
+      </c>
+      <c r="D52" s="5">
+        <v>70.491</v>
+      </c>
+      <c r="E52" s="22">
+        <f>D51/D52</f>
+        <v>0.76344497879161888</v>
+      </c>
+      <c r="F52" s="5">
+        <v>67.864999999999995</v>
+      </c>
+      <c r="G52" s="22">
+        <f>F51/F52</f>
+        <v>0.79292713475281817</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="15">
+      <c r="B53" s="24"/>
+      <c r="C53" s="17">
+        <v>4</v>
+      </c>
+      <c r="D53" s="5">
+        <v>110.785</v>
+      </c>
+      <c r="E53" s="22">
+        <f>D51/D53</f>
+        <v>0.48576973416978836</v>
+      </c>
+      <c r="F53" s="5">
+        <v>106.768</v>
+      </c>
+      <c r="G53" s="22">
+        <f>F51/F53</f>
+        <v>0.50400869174284424</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="15">
+      <c r="B54" s="24"/>
+      <c r="C54" s="17">
+        <v>8</v>
+      </c>
+      <c r="D54" s="5">
+        <v>216.523</v>
+      </c>
+      <c r="E54" s="22">
+        <f>D51/D54</f>
+        <v>0.24854634380643167</v>
+      </c>
+      <c r="F54" s="5">
+        <v>216.291</v>
+      </c>
+      <c r="G54" s="22">
+        <f>F51/F54</f>
+        <v>0.24879444822022181</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="15">
+      <c r="B55" s="24"/>
+      <c r="C55" s="17">
+        <v>16</v>
+      </c>
+      <c r="D55" s="5">
+        <v>494.69499999999999</v>
+      </c>
+      <c r="E55" s="22">
+        <f>D51/D55</f>
+        <v>0.10878622181344061</v>
+      </c>
+      <c r="F55" s="5">
+        <v>384.27330000000001</v>
+      </c>
+      <c r="G55" s="22">
+        <f>F51/F55</f>
+        <v>0.14003575059729623</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="15">
+      <c r="B56" s="24"/>
+      <c r="C56" s="17">
+        <v>32</v>
+      </c>
+      <c r="D56" s="5">
+        <v>986.30899999999997</v>
+      </c>
+      <c r="E56" s="22">
+        <f>D51/D56</f>
+        <v>5.4563022338841076E-2</v>
+      </c>
+      <c r="F56" s="5">
+        <v>789.94799999999998</v>
+      </c>
+      <c r="G56" s="22">
+        <f>F51/F56</f>
+        <v>6.8120939606151287E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="15.6" thickBot="1">
+      <c r="B57" s="24"/>
+      <c r="C57" s="18">
+        <v>64</v>
+      </c>
+      <c r="D57" s="9">
+        <v>1963.213</v>
+      </c>
+      <c r="E57" s="23">
+        <f>D51/D57</f>
+        <v>2.7412206418763529E-2</v>
+      </c>
+      <c r="F57" s="9">
+        <v>1952.7070000000001</v>
+      </c>
+      <c r="G57" s="23">
+        <f>F51/F57</f>
+        <v>2.7557641776262385E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -28663,44 +29270,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754D7C31-A8AA-4C0E-B26E-C4154CE576F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CF9564-1E6C-4AAE-878A-0E7D07362CD2}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="2" max="4" width="16.796875" customWidth="1"/>
+    <col min="5" max="5" width="16.796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="14.4" thickBot="1">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1">
       <c r="B2" s="20"/>
       <c r="C2" s="60" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="61"/>
-      <c r="E2" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="63"/>
     </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="24"/>
       <c r="B3" s="45" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>2</v>
@@ -28708,177 +29311,144 @@
       <c r="D3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="24"/>
       <c r="B4" s="42">
         <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>230.39099999999999</v>
+        <v>13.062200000000001</v>
       </c>
       <c r="D4" s="22">
         <f>C4/C4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>230.63399999999999</v>
-      </c>
-      <c r="F4" s="22">
-        <f>E4/E4</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="24"/>
       <c r="B5" s="43">
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>227.08199999999999</v>
+        <v>17.616099999999999</v>
       </c>
       <c r="D5" s="22">
         <f>C4/C5</f>
-        <v>1.0145718286786272</v>
-      </c>
-      <c r="E5" s="5">
-        <v>226.55</v>
-      </c>
-      <c r="F5" s="22">
-        <f>E4/E5</f>
-        <v>1.0180269256234826</v>
+        <v>0.74149215774206556</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="24"/>
       <c r="B6" s="43">
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>228.239</v>
+        <v>12.9846</v>
       </c>
       <c r="D6" s="22">
         <f>C4/C6</f>
-        <v>1.0094287128843011</v>
-      </c>
-      <c r="E6" s="5">
-        <v>228.81</v>
-      </c>
-      <c r="F6" s="22">
-        <f>E4/E6</f>
-        <v>1.0079716795594598</v>
+        <v>1.005976310398472</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="24"/>
       <c r="B7" s="43">
         <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>227.19499999999999</v>
+        <v>13.7319</v>
       </c>
       <c r="D7" s="22">
         <f>C4/C7</f>
-        <v>1.0140672109861573</v>
-      </c>
-      <c r="E7" s="5">
-        <v>226.61</v>
-      </c>
-      <c r="F7" s="22">
-        <f>E4/E7</f>
-        <v>1.0177573805216009</v>
+        <v>0.95123034685658947</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="24"/>
       <c r="B8" s="43">
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>234.80600000000001</v>
+        <v>15.492599999999999</v>
       </c>
       <c r="D8" s="22">
         <f>C4/C8</f>
-        <v>0.98119724368201822</v>
-      </c>
-      <c r="E8" s="5">
-        <v>227.22399999999999</v>
-      </c>
-      <c r="F8" s="22">
-        <f>E4/E8</f>
-        <v>1.0150072175474421</v>
+        <v>0.84312510488878567</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="24"/>
       <c r="B9" s="43">
         <v>32</v>
       </c>
       <c r="C9" s="4">
-        <v>236.06899999999999</v>
+        <v>26.883199999999999</v>
       </c>
       <c r="D9" s="22">
         <f>C4/C9</f>
-        <v>0.97594771020337279</v>
-      </c>
-      <c r="E9" s="5">
-        <v>231.97499999999999</v>
-      </c>
-      <c r="F9" s="22">
-        <f>E4/E9</f>
-        <v>0.99421920465567404</v>
+        <v>0.48588709677419362</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="24"/>
       <c r="B10" s="43">
         <v>64</v>
       </c>
       <c r="C10" s="4">
-        <v>241.56100000000001</v>
+        <v>54.066200000000002</v>
       </c>
       <c r="D10" s="22">
         <f>C4/C10</f>
-        <v>0.95375909190639208</v>
-      </c>
-      <c r="E10" s="5">
-        <v>237.21</v>
-      </c>
-      <c r="F10" s="22">
-        <f>E4/E10</f>
-        <v>0.97227772859491579</v>
+        <v>0.24159641328593465</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="15.6" thickBot="1">
       <c r="A11" s="24"/>
       <c r="B11" s="44">
         <v>128</v>
       </c>
       <c r="C11" s="8">
-        <v>248.33699999999999</v>
+        <v>20</v>
       </c>
       <c r="D11" s="23">
         <f>C4/C11</f>
-        <v>0.92773529518356102</v>
-      </c>
-      <c r="E11" s="9">
-        <v>247.124</v>
-      </c>
-      <c r="F11" s="23">
-        <f>E4/E11</f>
-        <v>0.93327236529029955</v>
-      </c>
+        <v>0.65311000000000008</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5">
+      <c r="E46"/>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47"/>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50"/>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52"/>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -28887,29 +29457,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CD3751-B357-4100-8733-3445447571DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C1B1DD-E39F-48FD-94EF-5C701A279DF2}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="6" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="14.4" thickBot="1">
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="30" customHeight="1" thickBot="1">
       <c r="B2" s="20"/>
       <c r="C2" s="51" t="s">
         <v>8</v>
@@ -28924,7 +29494,7 @@
       </c>
       <c r="H2" s="59"/>
     </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
         <v>7</v>
@@ -28948,174 +29518,174 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="24"/>
       <c r="B4" s="17">
         <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>226.73099999999999</v>
+        <v>27.9283</v>
       </c>
       <c r="D4" s="22">
         <f>C4/C4</f>
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>247.55099999999999</v>
+        <v>54.374299999999998</v>
       </c>
       <c r="F4" s="22">
         <f>E4/E4</f>
         <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>260.56700000000001</v>
+        <v>109.9502</v>
       </c>
       <c r="H4" s="21">
         <f>G4/G4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="24"/>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>227.59899999999999</v>
+        <v>34.0608</v>
       </c>
       <c r="D5" s="22">
         <f>C4/C5</f>
-        <v>0.99618627498363355</v>
+        <v>0.81995431698609544</v>
       </c>
       <c r="E5" s="5">
-        <v>231.38200000000001</v>
+        <v>67.715400000000002</v>
       </c>
       <c r="F5" s="22">
         <f>E4/E5</f>
-        <v>1.0698801116767942</v>
+        <v>0.80298277792053208</v>
       </c>
       <c r="G5" s="5">
-        <v>261.18400000000003</v>
+        <v>132.13669999999999</v>
       </c>
       <c r="H5" s="22">
         <f>G4/G5</f>
-        <v>0.99763768071551084</v>
+        <v>0.83209433866594218</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="24"/>
       <c r="B6" s="17">
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>227.459</v>
+        <v>34.138300000000001</v>
       </c>
       <c r="D6" s="22">
         <f>C4/C6</f>
-        <v>0.99679942319275117</v>
+        <v>0.81809287515781393</v>
       </c>
       <c r="E6" s="5">
-        <v>234.047</v>
+        <v>109.3655</v>
       </c>
       <c r="F6" s="22">
         <f>E4/E6</f>
-        <v>1.0576978128324652</v>
+        <v>0.49717964074593907</v>
       </c>
       <c r="G6" s="5">
-        <v>263.28500000000003</v>
+        <v>435.66809999999998</v>
       </c>
       <c r="H6" s="22">
         <f>G4/G6</f>
-        <v>0.98967658620886101</v>
+        <v>0.25237147268758031</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="24"/>
       <c r="B7" s="17">
         <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>235.167</v>
+        <v>32.020699999999998</v>
       </c>
       <c r="D7" s="22">
         <f>C4/C7</f>
-        <v>0.96412761994667617</v>
+        <v>0.87219517374698252</v>
       </c>
       <c r="E7" s="5">
-        <v>237.614</v>
+        <v>110.8036</v>
       </c>
       <c r="F7" s="22">
         <f>E4/E7</f>
-        <v>1.041819926435311</v>
+        <v>0.49072683559017932</v>
       </c>
       <c r="G7" s="5">
-        <v>267.54399999999998</v>
+        <v>440.1814</v>
       </c>
       <c r="H7" s="22">
         <f>G4/G7</f>
-        <v>0.97392204646712321</v>
+        <v>0.24978383911723664</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="24"/>
       <c r="B8" s="17">
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>234.31200000000001</v>
+        <v>54.841900000000003</v>
       </c>
       <c r="D8" s="22">
         <f>C4/C8</f>
-        <v>0.96764570316501064</v>
+        <v>0.50925113827201463</v>
       </c>
       <c r="E8" s="5">
-        <v>242.185</v>
+        <v>219.17310000000001</v>
       </c>
       <c r="F8" s="22">
         <f>E4/E8</f>
-        <v>1.0221566158102278</v>
+        <v>0.24808838310905854</v>
       </c>
       <c r="G8" s="5">
-        <v>292.45699999999999</v>
+        <v>874.27629999999999</v>
       </c>
       <c r="H8" s="22">
-        <f>G4/G8</f>
-        <v>0.89095832891672966</v>
+        <f>+G4/G8</f>
+        <v>0.12576138687506455</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="24"/>
       <c r="B9" s="17">
         <v>32</v>
       </c>
       <c r="C9" s="4">
-        <v>238.76300000000001</v>
+        <v>67.715400000000002</v>
       </c>
       <c r="D9" s="22">
         <f>C4/C9</f>
-        <v>0.94960693239739824</v>
+        <v>0.41243646201602591</v>
       </c>
       <c r="E9" s="5">
-        <v>241.512</v>
+        <v>399.65940000000001</v>
       </c>
       <c r="F9" s="22">
         <f>E4/E9</f>
-        <v>1.0250049686972076</v>
+        <v>0.1360515979356422</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="33"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="15.6" thickBot="1">
       <c r="A10" s="24"/>
       <c r="B10" s="18">
         <v>64</v>
       </c>
       <c r="C10" s="8">
-        <v>241.352</v>
+        <v>174.32409999999999</v>
       </c>
       <c r="D10" s="23">
         <f>C4/C10</f>
-        <v>0.93942043156882893</v>
+        <v>0.16020905887367268</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="30"/>

</xml_diff>